<commit_message>
docs: add team name on wbs
</commit_message>
<xml_diff>
--- a/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
+++ b/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GamesungCoding\2. Area\문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GamesungCoding\ResourceRepo\2.WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364E8539-5856-46D7-9327-FD4B59E367E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B82594-6CBE-4FBB-A346-401AADF0332B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
-  <si>
-    <t>팀명</t>
-  </si>
   <si>
     <t>구분</t>
   </si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>팀 전체</t>
+  </si>
+  <si>
+    <t>겜성코딩</t>
   </si>
 </sst>
 </file>
@@ -831,6 +831,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -838,15 +847,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1126,7 @@
   <sheetData>
     <row r="1" spans="1:60" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -1153,18 +1153,18 @@
     </row>
     <row r="2" spans="1:60" s="7" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="54" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="55"/>
       <c r="E2" s="55"/>
       <c r="F2" s="56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="57"/>
       <c r="H2" s="57"/>
@@ -1199,25 +1199,25 @@
     </row>
     <row r="3" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="C3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="D3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="E3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="F3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="G3" s="50" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>7</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1653,10 +1653,10 @@
     </row>
     <row r="5" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="45">
         <v>1</v>
@@ -1732,7 +1732,7 @@
     <row r="6" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
       <c r="B6" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="45">
         <v>1</v>
@@ -1804,7 +1804,7 @@
     <row r="7" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="48"/>
       <c r="B7" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="45">
         <v>1</v>
@@ -1876,7 +1876,7 @@
     <row r="8" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49"/>
       <c r="B8" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="45">
         <v>1</v>
@@ -1947,10 +1947,10 @@
     </row>
     <row r="9" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="45">
         <f>IF(COUNTBLANK(C10:C13)=4, "", SUM(C10:C13)/COUNT(C10:C13))</f>
@@ -2029,7 +2029,7 @@
     <row r="10" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="48"/>
       <c r="B10" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="45">
         <v>0.8</v>
@@ -2105,7 +2105,7 @@
     <row r="11" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="48"/>
       <c r="B11" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="45">
         <v>0</v>
@@ -2181,7 +2181,7 @@
     <row r="12" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
       <c r="B12" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="45">
         <v>0</v>
@@ -2258,7 +2258,7 @@
     <row r="13" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="45">
         <v>0</v>
@@ -2335,7 +2335,7 @@
     <row r="14" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
       <c r="B14" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="45">
         <f>IF(COUNTBLANK(C15:C18)=4, "", SUM(C15:C18)/COUNT(C15:C18))</f>
@@ -2414,7 +2414,7 @@
     <row r="15" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="48"/>
       <c r="B15" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="45">
         <v>0.05</v>
@@ -2488,7 +2488,7 @@
     <row r="16" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="48"/>
       <c r="B16" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="45">
         <v>0</v>
@@ -2564,7 +2564,7 @@
     <row r="17" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="48"/>
       <c r="B17" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="45">
         <v>0</v>
@@ -2640,7 +2640,7 @@
     <row r="18" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
       <c r="B18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="45">
         <v>0</v>
@@ -2716,7 +2716,7 @@
     <row r="19" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
       <c r="B19" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="45">
         <v>0</v>
@@ -2792,7 +2792,7 @@
     <row r="20" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
       <c r="B20" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="45">
         <f>IF(COUNTBLANK(C21:C22)=2, "", SUM(C21:C22)/COUNT(C21:C22))</f>
@@ -2871,7 +2871,7 @@
     <row r="21" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="48"/>
       <c r="B21" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="45">
         <v>0</v>
@@ -2947,7 +2947,7 @@
     <row r="22" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="48"/>
       <c r="B22" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="45">
         <v>0</v>
@@ -3023,7 +3023,7 @@
     <row r="23" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="48"/>
       <c r="B23" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="45">
         <f>IF(COUNTBLANK(C24:C25)=2, "", SUM(C24:C25)/COUNT(C24:C25))</f>
@@ -3102,7 +3102,7 @@
     <row r="24" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
       <c r="B24" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="45">
         <v>0</v>
@@ -3178,7 +3178,7 @@
     <row r="25" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
       <c r="B25" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="45">
         <v>0</v>
@@ -3254,7 +3254,7 @@
     <row r="26" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="48"/>
       <c r="B26" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="45">
         <f>IF(COUNTBLANK(C27:C28)=2, "", SUM(C27:C28)/COUNT(C27:C28))</f>
@@ -3333,7 +3333,7 @@
     <row r="27" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="48"/>
       <c r="B27" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="45">
         <v>0</v>
@@ -3409,7 +3409,7 @@
     <row r="28" spans="1:60" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="49"/>
       <c r="B28" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="45">
         <v>0</v>
@@ -7533,37 +7533,37 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4"/>
     </row>
@@ -7593,54 +7593,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="C1" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51"/>
-      <c r="B2" s="65"/>
+      <c r="B2" s="62"/>
       <c r="C2" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="F2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="G2" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="H2" s="42" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>23</v>
       </c>
       <c r="I2" s="42"/>
     </row>
     <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="43"/>
       <c r="D3" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
@@ -7651,11 +7651,11 @@
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="48"/>
       <c r="B4" s="38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
@@ -7666,11 +7666,11 @@
     <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48"/>
       <c r="B5" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="43"/>
       <c r="F5" s="43"/>
@@ -7681,11 +7681,11 @@
     <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
       <c r="B6" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
@@ -7695,26 +7695,26 @@
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="C7" s="64"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="48"/>
       <c r="B8" s="40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -7726,16 +7726,16 @@
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="48"/>
       <c r="B9" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="43"/>
       <c r="D9" s="43"/>
       <c r="E9" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="43"/>
       <c r="G9" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
@@ -7743,32 +7743,32 @@
     <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="48"/>
       <c r="B10" s="40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="43"/>
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I10" s="43"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="48"/>
       <c r="B11" s="40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="43"/>
       <c r="F11" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="43"/>
       <c r="H11" s="43"/>
@@ -7777,24 +7777,24 @@
     <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
       <c r="B12" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="63"/>
+        <v>28</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="66"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="43"/>
       <c r="F13" s="43"/>
@@ -7805,14 +7805,14 @@
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
       <c r="B14" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="43"/>
       <c r="G14" s="43"/>
@@ -7822,15 +7822,15 @@
     <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="48"/>
       <c r="B15" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="43"/>
       <c r="F15" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" s="43"/>
       <c r="H15" s="43"/>
@@ -7839,30 +7839,30 @@
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="48"/>
       <c r="B16" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="43"/>
       <c r="G16" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I16" s="43"/>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="48"/>
       <c r="B17" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="43"/>
       <c r="D17" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="43"/>
@@ -7873,23 +7873,23 @@
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
       <c r="B18" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="63"/>
+        <v>30</v>
+      </c>
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
       <c r="B19" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
@@ -7901,10 +7901,10 @@
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
       <c r="B20" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
@@ -7916,24 +7916,24 @@
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="48"/>
       <c r="B21" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
+        <v>31</v>
+      </c>
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="66"/>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="48"/>
       <c r="B22" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="43"/>
       <c r="D22" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="43"/>
       <c r="F22" s="43"/>
@@ -7944,10 +7944,10 @@
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="48"/>
       <c r="B23" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
@@ -7959,24 +7959,24 @@
     <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
       <c r="B24" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="63"/>
+        <v>40</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="66"/>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
       <c r="B25" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
@@ -7987,11 +7987,11 @@
     <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="49"/>
       <c r="B26" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="43"/>
       <c r="D26" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="43"/>
       <c r="F26" s="43"/>

</xml_diff>

<commit_message>
docs: update schedule on wbs
</commit_message>
<xml_diff>
--- a/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
+++ b/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GamesungCoding\ResourceRepo\2.WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278A3429-B1F5-4337-8680-3BA249E9418B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AC0F4E-0E0E-4F88-942E-BB3E6DFA5ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -858,9 +858,6 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -872,6 +869,15 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -912,13 +918,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -930,14 +936,8 @@
     <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1238,31 +1238,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
     </row>
     <row r="2" spans="1:67" s="7" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
@@ -1271,31 +1271,31 @@
       <c r="B2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="28"/>
@@ -1311,25 +1311,25 @@
       <c r="BC2" s="30"/>
     </row>
     <row r="3" spans="1:67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="53" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="8">
@@ -1573,13 +1573,13 @@
       </c>
     </row>
     <row r="4" spans="1:67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="9">
         <v>45951</v>
       </c>
@@ -1821,7 +1821,7 @@
       </c>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="51" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="18" t="s">
@@ -1850,10 +1850,10 @@
       <c r="K5" s="12"/>
       <c r="L5" s="32"/>
       <c r="M5" s="33"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="46"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="45"/>
       <c r="R5" s="12"/>
       <c r="S5" s="32"/>
       <c r="T5" s="33"/>
@@ -1906,7 +1906,7 @@
       <c r="BO5" s="12"/>
     </row>
     <row r="6" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
@@ -1929,10 +1929,10 @@
       <c r="K6" s="12"/>
       <c r="L6" s="32"/>
       <c r="M6" s="33"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="46"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="45"/>
       <c r="R6" s="12"/>
       <c r="S6" s="32"/>
       <c r="T6" s="33"/>
@@ -1985,7 +1985,7 @@
       <c r="BO6" s="12"/>
     </row>
     <row r="7" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="18" t="s">
         <v>10</v>
       </c>
@@ -2008,10 +2008,10 @@
       <c r="K7" s="12"/>
       <c r="L7" s="32"/>
       <c r="M7" s="33"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="46"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="45"/>
       <c r="R7" s="12"/>
       <c r="S7" s="32"/>
       <c r="T7" s="33"/>
@@ -2064,7 +2064,7 @@
       <c r="BO7" s="12"/>
     </row>
     <row r="8" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
@@ -2087,10 +2087,10 @@
       <c r="K8" s="12"/>
       <c r="L8" s="32"/>
       <c r="M8" s="33"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="46"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="45"/>
       <c r="R8" s="12"/>
       <c r="S8" s="32"/>
       <c r="T8" s="33"/>
@@ -2143,7 +2143,7 @@
       <c r="BO8" s="12"/>
     </row>
     <row r="9" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="48" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="41" t="s">
@@ -2175,10 +2175,10 @@
       <c r="K9" s="12"/>
       <c r="L9" s="32"/>
       <c r="M9" s="33"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="46"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="45"/>
       <c r="R9" s="12"/>
       <c r="S9" s="32"/>
       <c r="T9" s="33"/>
@@ -2231,7 +2231,7 @@
       <c r="BO9" s="12"/>
     </row>
     <row r="10" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="42" t="s">
         <v>23</v>
       </c>
@@ -2258,10 +2258,10 @@
       <c r="K10" s="12"/>
       <c r="L10" s="32"/>
       <c r="M10" s="33"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="46"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="45"/>
       <c r="R10" s="12"/>
       <c r="S10" s="32"/>
       <c r="T10" s="33"/>
@@ -2314,7 +2314,7 @@
       <c r="BO10" s="12"/>
     </row>
     <row r="11" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="42" t="s">
         <v>25</v>
       </c>
@@ -2341,10 +2341,10 @@
       <c r="K11" s="12"/>
       <c r="L11" s="32"/>
       <c r="M11" s="33"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="46"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="45"/>
       <c r="R11" s="12"/>
       <c r="S11" s="32"/>
       <c r="T11" s="33"/>
@@ -2397,7 +2397,7 @@
       <c r="BO11" s="12"/>
     </row>
     <row r="12" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="42" t="s">
         <v>52</v>
       </c>
@@ -2425,10 +2425,10 @@
       <c r="K12" s="12"/>
       <c r="L12" s="32"/>
       <c r="M12" s="33"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="46"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="45"/>
       <c r="R12" s="12"/>
       <c r="S12" s="32"/>
       <c r="T12" s="33"/>
@@ -2481,7 +2481,7 @@
       <c r="BO12" s="12"/>
     </row>
     <row r="13" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="41" t="s">
         <v>28</v>
       </c>
@@ -2511,10 +2511,10 @@
       <c r="K13" s="12"/>
       <c r="L13" s="32"/>
       <c r="M13" s="33"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="46"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="45"/>
       <c r="R13" s="12"/>
       <c r="S13" s="32"/>
       <c r="T13" s="33"/>
@@ -2567,7 +2567,7 @@
       <c r="BO13" s="12"/>
     </row>
     <row r="14" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="43" t="s">
         <v>32</v>
       </c>
@@ -2593,10 +2593,10 @@
       <c r="K14" s="12"/>
       <c r="L14" s="32"/>
       <c r="M14" s="33"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="46"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="45"/>
       <c r="R14" s="12"/>
       <c r="S14" s="32"/>
       <c r="T14" s="33"/>
@@ -2648,7 +2648,7 @@
       <c r="BO14" s="12"/>
     </row>
     <row r="15" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="43" t="s">
         <v>33</v>
       </c>
@@ -2675,10 +2675,10 @@
       <c r="K15" s="12"/>
       <c r="L15" s="32"/>
       <c r="M15" s="33"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="46"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="45"/>
       <c r="R15" s="12"/>
       <c r="S15" s="32"/>
       <c r="T15" s="33"/>
@@ -2731,7 +2731,7 @@
       <c r="BO15" s="12"/>
     </row>
     <row r="16" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="43" t="s">
         <v>34</v>
       </c>
@@ -2758,10 +2758,10 @@
       <c r="K16" s="12"/>
       <c r="L16" s="32"/>
       <c r="M16" s="33"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="46"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="45"/>
       <c r="R16" s="12"/>
       <c r="S16" s="32"/>
       <c r="T16" s="33"/>
@@ -2814,7 +2814,7 @@
       <c r="BO16" s="12"/>
     </row>
     <row r="17" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="43" t="s">
         <v>35</v>
       </c>
@@ -2841,10 +2841,10 @@
       <c r="K17" s="12"/>
       <c r="L17" s="32"/>
       <c r="M17" s="33"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="46"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="45"/>
       <c r="R17" s="12"/>
       <c r="S17" s="32"/>
       <c r="T17" s="33"/>
@@ -2897,7 +2897,7 @@
       <c r="BO17" s="12"/>
     </row>
     <row r="18" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="41" t="s">
         <v>29</v>
       </c>
@@ -2924,10 +2924,10 @@
       <c r="K18" s="12"/>
       <c r="L18" s="32"/>
       <c r="M18" s="33"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="46"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="45"/>
       <c r="R18" s="12"/>
       <c r="S18" s="32"/>
       <c r="T18" s="33"/>
@@ -2980,7 +2980,7 @@
       <c r="BO18" s="12"/>
     </row>
     <row r="19" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="41" t="s">
         <v>30</v>
       </c>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="D19" s="10">
         <f>IF(AND(F19&lt;&gt;"", E19&lt;&gt;""), F19-E19+1, "")</f>
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E19" s="11">
         <f>IF(COUNTA(E20:E21)=0,"", MIN(E20:E21))</f>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="F19" s="11">
         <f>IF(COUNTBLANK(F20:F21)=2,"", MAX(F20:F21))</f>
-        <v>46000</v>
+        <v>45996</v>
       </c>
       <c r="G19" s="38" t="str" cm="1">
         <f t="array" ref="G19">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C18:I18="O", 담당자!C$2:I$2, ""))</f>
@@ -3010,10 +3010,10 @@
       <c r="K19" s="12"/>
       <c r="L19" s="32"/>
       <c r="M19" s="33"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="46"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="45"/>
       <c r="R19" s="12"/>
       <c r="S19" s="32"/>
       <c r="T19" s="33"/>
@@ -3066,7 +3066,7 @@
       <c r="BO19" s="12"/>
     </row>
     <row r="20" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="43" t="s">
         <v>36</v>
       </c>
@@ -3074,14 +3074,14 @@
         <v>0</v>
       </c>
       <c r="D20" s="10">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E20" s="11">
         <v>45966</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="10"/>
-        <v>46000</v>
+        <v>45996</v>
       </c>
       <c r="G20" s="36" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C19:I19="O", 담당자!C$2:I$2, ""))</f>
@@ -3093,10 +3093,10 @@
       <c r="K20" s="12"/>
       <c r="L20" s="32"/>
       <c r="M20" s="33"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="46"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="45"/>
       <c r="R20" s="12"/>
       <c r="S20" s="32"/>
       <c r="T20" s="33"/>
@@ -3149,7 +3149,7 @@
       <c r="BO20" s="12"/>
     </row>
     <row r="21" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="43" t="s">
         <v>37</v>
       </c>
@@ -3157,14 +3157,14 @@
         <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E21" s="11">
         <v>45966</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" si="10"/>
-        <v>46000</v>
+        <v>45996</v>
       </c>
       <c r="G21" s="36" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C20:I20="O", 담당자!C$2:I$2, ""))</f>
@@ -3176,10 +3176,10 @@
       <c r="K21" s="12"/>
       <c r="L21" s="32"/>
       <c r="M21" s="33"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="46"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="45"/>
       <c r="R21" s="12"/>
       <c r="S21" s="32"/>
       <c r="T21" s="33"/>
@@ -3232,7 +3232,7 @@
       <c r="BO21" s="12"/>
     </row>
     <row r="22" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="41" t="s">
         <v>31</v>
       </c>
@@ -3242,15 +3242,15 @@
       </c>
       <c r="D22" s="10">
         <f>IF(AND(F22&lt;&gt;"", E22&lt;&gt;""), F22-E22+1, "")</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E22" s="11">
         <f>IF(COUNTA(E23:E24)=0,"", MIN(E23:E24))</f>
-        <v>46000</v>
+        <v>45997</v>
       </c>
       <c r="F22" s="11">
         <f>IF(COUNTBLANK(F23:F24)=2,"", MAX(F23:F24))</f>
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="G22" s="38" t="str" cm="1">
         <f t="array" ref="G22">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C21:I21="O", 담당자!C$2:I$2, ""))</f>
@@ -3262,10 +3262,10 @@
       <c r="K22" s="12"/>
       <c r="L22" s="32"/>
       <c r="M22" s="33"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="48"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="46"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="45"/>
       <c r="R22" s="12"/>
       <c r="S22" s="32"/>
       <c r="T22" s="33"/>
@@ -3318,7 +3318,7 @@
       <c r="BO22" s="12"/>
     </row>
     <row r="23" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="43" t="s">
         <v>38</v>
       </c>
@@ -3326,14 +3326,14 @@
         <v>0</v>
       </c>
       <c r="D23" s="10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E23" s="11">
-        <v>46000</v>
+        <v>45997</v>
       </c>
       <c r="F23" s="11">
         <f t="shared" si="10"/>
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="G23" s="36" t="str" cm="1">
         <f t="array" ref="G23">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C22:I22="O", 담당자!C$2:I$2, ""))</f>
@@ -3345,10 +3345,10 @@
       <c r="K23" s="12"/>
       <c r="L23" s="32"/>
       <c r="M23" s="33"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="46"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="45"/>
       <c r="R23" s="12"/>
       <c r="S23" s="32"/>
       <c r="T23" s="33"/>
@@ -3401,7 +3401,7 @@
       <c r="BO23" s="12"/>
     </row>
     <row r="24" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="43" t="s">
         <v>39</v>
       </c>
@@ -3409,14 +3409,14 @@
         <v>0</v>
       </c>
       <c r="D24" s="10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E24" s="11">
-        <v>46000</v>
+        <v>45997</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" si="10"/>
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="G24" s="36" t="str" cm="1">
         <f t="array" ref="G24">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C23:I23="O", 담당자!C$2:I$2, ""))</f>
@@ -3428,10 +3428,10 @@
       <c r="K24" s="40"/>
       <c r="L24" s="32"/>
       <c r="M24" s="33"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="46"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="45"/>
       <c r="R24" s="12"/>
       <c r="S24" s="32"/>
       <c r="T24" s="33"/>
@@ -3484,7 +3484,7 @@
       <c r="BO24" s="12"/>
     </row>
     <row r="25" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="41" t="s">
         <v>40</v>
       </c>
@@ -3494,15 +3494,15 @@
       </c>
       <c r="D25" s="10">
         <f>IF(AND(F25&lt;&gt;"", E25&lt;&gt;""), F25-E25+1, "")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E25" s="11">
         <f>IF(COUNTA(E26:E27)=0,"", MIN(E26:E27))</f>
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="F25" s="11">
         <f>IF(COUNTBLANK(F26:F27)=2,"", MAX(F26:F27))</f>
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="G25" s="38" t="str" cm="1">
         <f t="array" ref="G25">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C24:I24="O", 담당자!C$2:I$2, ""))</f>
@@ -3514,10 +3514,10 @@
       <c r="K25" s="12"/>
       <c r="L25" s="32"/>
       <c r="M25" s="33"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="48"/>
-      <c r="Q25" s="46"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="45"/>
       <c r="R25" s="12"/>
       <c r="S25" s="32"/>
       <c r="T25" s="33"/>
@@ -3570,7 +3570,7 @@
       <c r="BO25" s="12"/>
     </row>
     <row r="26" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="63"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="43" t="s">
         <v>41</v>
       </c>
@@ -3578,14 +3578,14 @@
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E26" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="F26" s="11">
         <f t="shared" si="10"/>
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="G26" s="36" t="str" cm="1">
         <f t="array" ref="G26">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C25:I25="O", 담당자!C$2:I$2, ""))</f>
@@ -3597,10 +3597,10 @@
       <c r="K26" s="12"/>
       <c r="L26" s="32"/>
       <c r="M26" s="33"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="48"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="46"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="45"/>
       <c r="R26" s="12"/>
       <c r="S26" s="32"/>
       <c r="T26" s="33"/>
@@ -3653,7 +3653,7 @@
       <c r="BO26" s="12"/>
     </row>
     <row r="27" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="43" t="s">
         <v>42</v>
       </c>
@@ -3661,14 +3661,14 @@
         <v>0</v>
       </c>
       <c r="D27" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E27" s="11">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="F27" s="11">
         <f t="shared" si="10"/>
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="G27" s="36" t="str" cm="1">
         <f t="array" ref="G27">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C26:I26="O", 담당자!C$2:I$2, ""))</f>
@@ -3680,10 +3680,10 @@
       <c r="K27" s="12"/>
       <c r="L27" s="32"/>
       <c r="M27" s="33"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="48"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="46"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="45"/>
       <c r="R27" s="12"/>
       <c r="S27" s="32"/>
       <c r="T27" s="33"/>
@@ -3736,7 +3736,7 @@
       <c r="BO27" s="12"/>
     </row>
     <row r="28" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="63"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="41" t="s">
         <v>47</v>
       </c>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="D28" s="10">
         <f>IF(AND(F28&lt;&gt;"", E28&lt;&gt;""), F28-E28+1, "")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="11">
         <f>IF(COUNTA(E29:E30)=0,"", MIN(E29:E30))</f>
@@ -3754,7 +3754,7 @@
       </c>
       <c r="F28" s="11">
         <f>IF(COUNTBLANK(F29:F30)=2,"", MAX(F29:F30))</f>
-        <v>46010</v>
+        <v>46009</v>
       </c>
       <c r="G28" s="38" t="str" cm="1">
         <f t="array" ref="G28">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C24:I24="O", 담당자!C$2:I$2, ""))</f>
@@ -3766,10 +3766,10 @@
       <c r="K28" s="12"/>
       <c r="L28" s="32"/>
       <c r="M28" s="33"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="46"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="45"/>
       <c r="R28" s="12"/>
       <c r="S28" s="32"/>
       <c r="T28" s="33"/>
@@ -3822,7 +3822,7 @@
       <c r="BO28" s="12"/>
     </row>
     <row r="29" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="63"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="43" t="s">
         <v>48</v>
       </c>
@@ -3830,14 +3830,14 @@
         <v>0</v>
       </c>
       <c r="D29" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" s="11">
         <v>46006</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" si="10"/>
-        <v>46010</v>
+        <v>46009</v>
       </c>
       <c r="G29" s="36" t="str" cm="1">
         <f t="array" ref="G29">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C28:I28="O", 담당자!C$2:I$2, ""))</f>
@@ -3849,10 +3849,10 @@
       <c r="K29" s="12"/>
       <c r="L29" s="32"/>
       <c r="M29" s="33"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="46"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="45"/>
       <c r="R29" s="12"/>
       <c r="S29" s="32"/>
       <c r="T29" s="33"/>
@@ -3905,7 +3905,7 @@
       <c r="BO29" s="12"/>
     </row>
     <row r="30" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="63"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="43" t="s">
         <v>49</v>
       </c>
@@ -3913,14 +3913,14 @@
         <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" s="11">
         <v>46006</v>
       </c>
       <c r="F30" s="11">
         <f t="shared" si="10"/>
-        <v>46010</v>
+        <v>46009</v>
       </c>
       <c r="G30" s="36" t="str" cm="1">
         <f t="array" ref="G30">_xlfn.TEXTJOIN(", ", TRUE, IF(담당자!C29:I29="O", 담당자!C$2:I$2, ""))</f>
@@ -3932,10 +3932,10 @@
       <c r="K30" s="12"/>
       <c r="L30" s="32"/>
       <c r="M30" s="33"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="46"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="45"/>
       <c r="R30" s="12"/>
       <c r="S30" s="32"/>
       <c r="T30" s="33"/>
@@ -3988,7 +3988,7 @@
       <c r="BO30" s="12"/>
     </row>
     <row r="31" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="63"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="41" t="s">
         <v>50</v>
       </c>
@@ -4018,10 +4018,10 @@
       <c r="K31" s="12"/>
       <c r="L31" s="32"/>
       <c r="M31" s="33"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="46"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="47"/>
+      <c r="P31" s="47"/>
+      <c r="Q31" s="45"/>
       <c r="R31" s="12"/>
       <c r="S31" s="32"/>
       <c r="T31" s="33"/>
@@ -4074,7 +4074,7 @@
       <c r="BO31" s="12"/>
     </row>
     <row r="32" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="64"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="43" t="s">
         <v>51</v>
       </c>
@@ -4101,10 +4101,10 @@
       <c r="K32" s="12"/>
       <c r="L32" s="32"/>
       <c r="M32" s="33"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="48"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="46"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="45"/>
       <c r="R32" s="12"/>
       <c r="S32" s="32"/>
       <c r="T32" s="33"/>
@@ -4166,10 +4166,10 @@
       <c r="L33" s="22"/>
       <c r="M33" s="26"/>
       <c r="N33" s="13"/>
-      <c r="O33" s="44" t="s">
+      <c r="O33" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="P33" s="44"/>
+      <c r="P33" s="70"/>
       <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
       <c r="S33" s="22"/>
@@ -8222,25 +8222,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="66"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="34" t="s">
         <v>44</v>
       </c>
@@ -8262,7 +8262,7 @@
       <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="51" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -8279,7 +8279,7 @@
       <c r="I3" s="35"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="50"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="18" t="s">
         <v>9</v>
       </c>
@@ -8294,7 +8294,7 @@
       <c r="I4" s="35"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
@@ -8309,7 +8309,7 @@
       <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
@@ -8324,22 +8324,22 @@
       <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="48" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="70"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="42" t="s">
         <v>23</v>
       </c>
@@ -8354,7 +8354,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="42" t="s">
         <v>25</v>
       </c>
@@ -8371,7 +8371,7 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="42" t="s">
         <v>26</v>
       </c>
@@ -8388,7 +8388,7 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="42" t="s">
         <v>27</v>
       </c>
@@ -8405,20 +8405,20 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="70"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="66"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="43" t="s">
         <v>32</v>
       </c>
@@ -8433,7 +8433,7 @@
       <c r="I13" s="35"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="43" t="s">
         <v>33</v>
       </c>
@@ -8450,7 +8450,7 @@
       <c r="I14" s="35"/>
     </row>
     <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="43" t="s">
         <v>34</v>
       </c>
@@ -8467,7 +8467,7 @@
       <c r="I15" s="35"/>
     </row>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="43" t="s">
         <v>35</v>
       </c>
@@ -8486,7 +8486,7 @@
       <c r="I16" s="35"/>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="41" t="s">
         <v>29</v>
       </c>
@@ -8501,20 +8501,20 @@
       <c r="I17" s="35"/>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="70"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="43" t="s">
         <v>36</v>
       </c>
@@ -8529,7 +8529,7 @@
       <c r="I19" s="35"/>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="43" t="s">
         <v>37</v>
       </c>
@@ -8544,20 +8544,20 @@
       <c r="I20" s="35"/>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="70"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="66"/>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="43" t="s">
         <v>38</v>
       </c>
@@ -8572,7 +8572,7 @@
       <c r="I22" s="35"/>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="43" t="s">
         <v>39</v>
       </c>
@@ -8587,20 +8587,20 @@
       <c r="I23" s="35"/>
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="70"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="66"/>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="43" t="s">
         <v>41</v>
       </c>
@@ -8615,7 +8615,7 @@
       <c r="I25" s="35"/>
     </row>
     <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="63"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="43" t="s">
         <v>42</v>
       </c>
@@ -8630,20 +8630,20 @@
       <c r="I26" s="35"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="70"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="66"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="63"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="43" t="s">
         <v>48</v>
       </c>
@@ -8658,7 +8658,7 @@
       <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="63"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="43" t="s">
         <v>49</v>
       </c>
@@ -8673,20 +8673,20 @@
       <c r="I29" s="35"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="63"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="70"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="66"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="63"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="43" t="s">
         <v>41</v>
       </c>
@@ -8701,7 +8701,7 @@
       <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="64"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="43" t="s">
         <v>42</v>
       </c>
@@ -8717,6 +8717,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C12:I12"/>
@@ -8724,11 +8729,6 @@
     <mergeCell ref="A7:A32"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="C30:I30"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
docs: update Oct. 5w journal and wbs progress
</commit_message>
<xml_diff>
--- a/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
+++ b/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GamesungCoding\ResourceRepo\2.WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AC0F4E-0E0E-4F88-942E-BB3E6DFA5ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DEEB81-CEF7-4E5D-9F6D-EB97E2F9FCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,6 +870,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -918,15 +921,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -936,8 +930,14 @@
     <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1238,31 +1238,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
     </row>
     <row r="2" spans="1:67" s="7" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
@@ -1271,31 +1271,31 @@
       <c r="B2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="59" t="s">
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="28"/>
@@ -1311,25 +1311,25 @@
       <c r="BC2" s="30"/>
     </row>
     <row r="3" spans="1:67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="54" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="8">
@@ -1573,13 +1573,13 @@
       </c>
     </row>
     <row r="4" spans="1:67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="9">
         <v>45951</v>
       </c>
@@ -1821,7 +1821,7 @@
       </c>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="18" t="s">
@@ -1906,7 +1906,7 @@
       <c r="BO5" s="12"/>
     </row>
     <row r="6" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="BO6" s="12"/>
     </row>
     <row r="7" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="18" t="s">
         <v>10</v>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="BO7" s="12"/>
     </row>
     <row r="8" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="BO8" s="12"/>
     </row>
     <row r="9" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="49" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="41" t="s">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="C9" s="37">
         <f>IF(COUNTBLANK(C10:C12)=4, "", SUM(C10:C12)/COUNT(C10:C12))</f>
-        <v>0.26666666666666666</v>
+        <v>0.93333333333333324</v>
       </c>
       <c r="D9" s="10">
         <f>IF(AND(F9&lt;&gt;"", E9&lt;&gt;""), F9-E9+1, "")</f>
@@ -2231,12 +2231,12 @@
       <c r="BO9" s="12"/>
     </row>
     <row r="10" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="49"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="42" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="37">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D10" s="10">
         <v>4</v>
@@ -2314,12 +2314,12 @@
       <c r="BO10" s="12"/>
     </row>
     <row r="11" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="37">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D11" s="10">
         <v>2</v>
@@ -2397,12 +2397,12 @@
       <c r="BO11" s="12"/>
     </row>
     <row r="12" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="42" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="10">
         <v>2</v>
@@ -2481,13 +2481,13 @@
       <c r="BO12" s="12"/>
     </row>
     <row r="13" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="41" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="37">
         <f>IF(COUNTBLANK(C14:C17)=4, "", SUM(C14:C17)/COUNT(C14:C17))</f>
-        <v>1.2500000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D13" s="10">
         <f>IF(AND(F13&lt;&gt;"", E13&lt;&gt;""), F13-E13+1, "")</f>
@@ -2567,12 +2567,12 @@
       <c r="BO13" s="12"/>
     </row>
     <row r="14" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="43" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="37">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D14" s="10">
         <v>4</v>
@@ -2648,7 +2648,7 @@
       <c r="BO14" s="12"/>
     </row>
     <row r="15" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="43" t="s">
         <v>33</v>
       </c>
@@ -2731,7 +2731,7 @@
       <c r="BO15" s="12"/>
     </row>
     <row r="16" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="43" t="s">
         <v>34</v>
       </c>
@@ -2814,7 +2814,7 @@
       <c r="BO16" s="12"/>
     </row>
     <row r="17" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="43" t="s">
         <v>35</v>
       </c>
@@ -2897,7 +2897,7 @@
       <c r="BO17" s="12"/>
     </row>
     <row r="18" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="49"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="41" t="s">
         <v>29</v>
       </c>
@@ -2980,7 +2980,7 @@
       <c r="BO18" s="12"/>
     </row>
     <row r="19" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="49"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="41" t="s">
         <v>30</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="BO19" s="12"/>
     </row>
     <row r="20" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="43" t="s">
         <v>36</v>
       </c>
@@ -3149,7 +3149,7 @@
       <c r="BO20" s="12"/>
     </row>
     <row r="21" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="43" t="s">
         <v>37</v>
       </c>
@@ -3232,7 +3232,7 @@
       <c r="BO21" s="12"/>
     </row>
     <row r="22" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="41" t="s">
         <v>31</v>
       </c>
@@ -3318,7 +3318,7 @@
       <c r="BO22" s="12"/>
     </row>
     <row r="23" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="43" t="s">
         <v>38</v>
       </c>
@@ -3401,7 +3401,7 @@
       <c r="BO23" s="12"/>
     </row>
     <row r="24" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="43" t="s">
         <v>39</v>
       </c>
@@ -3484,7 +3484,7 @@
       <c r="BO24" s="12"/>
     </row>
     <row r="25" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="41" t="s">
         <v>40</v>
       </c>
@@ -3570,7 +3570,7 @@
       <c r="BO25" s="12"/>
     </row>
     <row r="26" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="43" t="s">
         <v>41</v>
       </c>
@@ -3653,7 +3653,7 @@
       <c r="BO26" s="12"/>
     </row>
     <row r="27" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="43" t="s">
         <v>42</v>
       </c>
@@ -3736,7 +3736,7 @@
       <c r="BO27" s="12"/>
     </row>
     <row r="28" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="41" t="s">
         <v>47</v>
       </c>
@@ -3822,7 +3822,7 @@
       <c r="BO28" s="12"/>
     </row>
     <row r="29" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="43" t="s">
         <v>48</v>
       </c>
@@ -3905,7 +3905,7 @@
       <c r="BO29" s="12"/>
     </row>
     <row r="30" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="43" t="s">
         <v>49</v>
       </c>
@@ -3988,7 +3988,7 @@
       <c r="BO30" s="12"/>
     </row>
     <row r="31" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="41" t="s">
         <v>50</v>
       </c>
@@ -4074,7 +4074,7 @@
       <c r="BO31" s="12"/>
     </row>
     <row r="32" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="50"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="43" t="s">
         <v>51</v>
       </c>
@@ -4166,10 +4166,10 @@
       <c r="L33" s="22"/>
       <c r="M33" s="26"/>
       <c r="N33" s="13"/>
-      <c r="O33" s="70" t="s">
+      <c r="O33" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="P33" s="70"/>
+      <c r="P33" s="48"/>
       <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
       <c r="S33" s="22"/>
@@ -8222,25 +8222,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
-      <c r="B2" s="68"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="66"/>
       <c r="C2" s="34" t="s">
         <v>44</v>
       </c>
@@ -8262,7 +8262,7 @@
       <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -8279,7 +8279,7 @@
       <c r="I3" s="35"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="18" t="s">
         <v>9</v>
       </c>
@@ -8294,7 +8294,7 @@
       <c r="I4" s="35"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
@@ -8309,7 +8309,7 @@
       <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
@@ -8324,22 +8324,22 @@
       <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="49" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="66"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="70"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="49"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="42" t="s">
         <v>23</v>
       </c>
@@ -8354,7 +8354,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="42" t="s">
         <v>25</v>
       </c>
@@ -8371,7 +8371,7 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="49"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="42" t="s">
         <v>26</v>
       </c>
@@ -8388,7 +8388,7 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="42" t="s">
         <v>27</v>
       </c>
@@ -8405,20 +8405,20 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="66"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="70"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="43" t="s">
         <v>32</v>
       </c>
@@ -8433,7 +8433,7 @@
       <c r="I13" s="35"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="43" t="s">
         <v>33</v>
       </c>
@@ -8450,7 +8450,7 @@
       <c r="I14" s="35"/>
     </row>
     <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="43" t="s">
         <v>34</v>
       </c>
@@ -8467,7 +8467,7 @@
       <c r="I15" s="35"/>
     </row>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="43" t="s">
         <v>35</v>
       </c>
@@ -8486,7 +8486,7 @@
       <c r="I16" s="35"/>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="41" t="s">
         <v>29</v>
       </c>
@@ -8501,20 +8501,20 @@
       <c r="I17" s="35"/>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="49"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="66"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="49"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="43" t="s">
         <v>36</v>
       </c>
@@ -8529,7 +8529,7 @@
       <c r="I19" s="35"/>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="43" t="s">
         <v>37</v>
       </c>
@@ -8544,20 +8544,20 @@
       <c r="I20" s="35"/>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="66"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="70"/>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="43" t="s">
         <v>38</v>
       </c>
@@ -8572,7 +8572,7 @@
       <c r="I22" s="35"/>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="43" t="s">
         <v>39</v>
       </c>
@@ -8587,20 +8587,20 @@
       <c r="I23" s="35"/>
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="70"/>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="43" t="s">
         <v>41</v>
       </c>
@@ -8615,7 +8615,7 @@
       <c r="I25" s="35"/>
     </row>
     <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="43" t="s">
         <v>42</v>
       </c>
@@ -8630,20 +8630,20 @@
       <c r="I26" s="35"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="66"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="70"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="43" t="s">
         <v>48</v>
       </c>
@@ -8658,7 +8658,7 @@
       <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="43" t="s">
         <v>49</v>
       </c>
@@ -8673,20 +8673,20 @@
       <c r="I29" s="35"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="64"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="66"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="70"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="43" t="s">
         <v>41</v>
       </c>
@@ -8701,7 +8701,7 @@
       <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="50"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="43" t="s">
         <v>42</v>
       </c>
@@ -8717,11 +8717,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C12:I12"/>
@@ -8729,6 +8724,11 @@
     <mergeCell ref="A7:A32"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="C30:I30"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
refactor: convert to markdown
- 작성 편의성을 위해 `docx` 파일을 `.md`로 수정
- 각 디렉토리에 `README.md`를 작성하여 문서 Hyperlink 연결
</commit_message>
<xml_diff>
--- a/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
+++ b/2.WBS/WBS_현대이지웰_최종프로젝트.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GamesungCoding\ResourceRepo\2.WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DEEB81-CEF7-4E5D-9F6D-EB97E2F9FCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7F2796-9D0E-4DF0-96BB-6D0452D56202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -921,6 +921,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,15 +937,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="C9" s="37">
         <f>IF(COUNTBLANK(C10:C12)=4, "", SUM(C10:C12)/COUNT(C10:C12))</f>
-        <v>0.93333333333333324</v>
+        <v>1</v>
       </c>
       <c r="D9" s="10">
         <f>IF(AND(F9&lt;&gt;"", E9&lt;&gt;""), F9-E9+1, "")</f>
@@ -2319,7 +2319,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="37">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D11" s="10">
         <v>2</v>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="C13" s="37">
         <f>IF(COUNTBLANK(C14:C17)=4, "", SUM(C14:C17)/COUNT(C14:C17))</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.85</v>
       </c>
       <c r="D13" s="10">
         <f>IF(AND(F13&lt;&gt;"", E13&lt;&gt;""), F13-E13+1, "")</f>
@@ -2572,7 +2572,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="37">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D14" s="10">
         <v>4</v>
@@ -2653,7 +2653,7 @@
         <v>33</v>
       </c>
       <c r="C15" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="10">
         <v>4</v>
@@ -2736,7 +2736,7 @@
         <v>34</v>
       </c>
       <c r="C16" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="10">
         <v>5</v>
@@ -2819,7 +2819,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="37">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D17" s="10">
         <v>15</v>
@@ -2902,7 +2902,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="37">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D18" s="10">
         <v>1</v>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="C19" s="37">
         <f>IF(COUNTBLANK(C20:C21)=2, "", SUM(C20:C21)/COUNT(C20:C21))</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D19" s="10">
         <f>IF(AND(F19&lt;&gt;"", E19&lt;&gt;""), F19-E19+1, "")</f>
@@ -3071,7 +3071,7 @@
         <v>36</v>
       </c>
       <c r="C20" s="37">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D20" s="10">
         <v>31</v>
@@ -8225,22 +8225,22 @@
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="55"/>
-      <c r="B2" s="66"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="34" t="s">
         <v>44</v>
       </c>
@@ -8330,13 +8330,13 @@
       <c r="B7" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="70"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="67"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="50"/>
@@ -8409,13 +8409,13 @@
       <c r="B12" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="70"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="67"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="50"/>
@@ -8505,13 +8505,13 @@
       <c r="B18" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="70"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="67"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
@@ -8548,13 +8548,13 @@
       <c r="B21" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="70"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="67"/>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="50"/>
@@ -8591,13 +8591,13 @@
       <c r="B24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="70"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="50"/>
@@ -8634,13 +8634,13 @@
       <c r="B27" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="70"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="67"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="50"/>
@@ -8677,13 +8677,13 @@
       <c r="B30" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="70"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="67"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="50"/>
@@ -8717,6 +8717,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C12:I12"/>
@@ -8724,11 +8729,6 @@
     <mergeCell ref="A7:A32"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="C30:I30"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>